<commit_message>
Commited code with complete flow
</commit_message>
<xml_diff>
--- a/src/test/java/com/comcast/orderlab/testdata/testdata.xlsx
+++ b/src/test/java/com/comcast/orderlab/testdata/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\maven\MavenOrderLab\src\test\java\com\comcast\orderlab\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\maven\RetailUi\src\test\java\com\comcast\orderlab\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="84">
   <si>
     <t>Y</t>
   </si>
@@ -251,12 +251,6 @@
     <t>102 DRCSG116055RES RD</t>
   </si>
   <si>
-    <t>103 DRCSG116055RES RD</t>
-  </si>
-  <si>
-    <t>104 DRCSG116055RES RD</t>
-  </si>
-  <si>
     <t>CreateDataOnlyAccounts</t>
   </si>
   <si>
@@ -266,7 +260,61 @@
     <t>y</t>
   </si>
   <si>
+    <t>107 DRCSG116054RES RD</t>
+  </si>
+  <si>
+    <t>108 DRCSG116054RES RD</t>
+  </si>
+  <si>
+    <t>109 DRCSG116054RES RD</t>
+  </si>
+  <si>
     <t>dgopin003c</t>
+  </si>
+  <si>
+    <t>23223</t>
+  </si>
+  <si>
+    <t>salutation</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>ssn</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>cvv</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
@@ -371,7 +419,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -391,6 +439,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -694,15 +745,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -720,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +797,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
@@ -755,52 +806,52 @@
         <v>10</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="1">
-        <v>23223</v>
+        <v>65</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -842,112 +893,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="1">
-        <v>23223</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="K2" r:id="rId3"/>
-    <hyperlink ref="I2" r:id="rId4"/>
-    <hyperlink ref="K4" r:id="rId5"/>
-    <hyperlink ref="I4" r:id="rId6"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -957,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +926,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1343,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A16" sqref="A16:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,6 +1585,152 @@
         <v>41</v>
       </c>
     </row>
+    <row r="16" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1"/>
@@ -1646,6 +1741,12 @@
     <hyperlink ref="O3" r:id="rId6"/>
     <hyperlink ref="O4" r:id="rId7"/>
     <hyperlink ref="O5" r:id="rId8"/>
+    <hyperlink ref="K18" r:id="rId9"/>
+    <hyperlink ref="I18" r:id="rId10"/>
+    <hyperlink ref="K16" r:id="rId11"/>
+    <hyperlink ref="I16" r:id="rId12"/>
+    <hyperlink ref="K17" r:id="rId13"/>
+    <hyperlink ref="I17" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>